<commit_message>
[fix] fix error from market and orders and refactor extract card data
</commit_message>
<xml_diff>
--- a/flask/static/data/result/categories.xlsx
+++ b/flask/static/data/result/categories.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,55 +448,55 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>communication</t>
+          <t>category_shopping</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>통신,KT,SKT,LGU+</t>
+          <t>백화점,마트/편의점,온라인쇼핑,소셜커머스,해외직구,홈쇼핑,SPA브랜드,아울렛,대형마트,SSM,전통시장,면세점,모든가맹점,국내외가맹점,화장품,드럭스토어</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>shopping</t>
+          <t>category_culture</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>백화점,마트/편의점,온라인쇼핑,소셜커머스,해외직구,온라인 여행사,홈쇼핑,SPA브랜드,아울렛,대형마트,SSM,전통시장,면세점,모든가맹점,국내외가맹점</t>
+          <t>영화,공연/전시,문화센터,도서,음원사이트,영화/문화,디지털구독,골프</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>culture</t>
+          <t>category_transportation</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>영화,공연/전시,문화센터,도서,음원사이트,영화/문화,디지털구독</t>
+          <t>고속버스,항공권,기차,대중교통,렌터카,택시,교통</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>transportation</t>
+          <t>category_car</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>고속버스,저가항공,항공권,기차,대중교통,렌터카,택시,자동차/하이패스,하이패스,충전소,교통</t>
+          <t>주유,자동차,정비,주유소,충전소,하이패스,자동차/하이패스</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>food</t>
+          <t>category_food</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>category_education</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,48 +520,60 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>utilities</t>
+          <t>category_housing_communication</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>공과금,공과금/렌탈</t>
+          <t>공과금,공과금/렌탈,통신,KT,SKT,LGU+</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>aviation</t>
+          <t>category_travel</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>진에어,대한항공,아시아나항공,제주항공,항공마일리지</t>
+          <t>진에어,대한항공,아시아나항공,제주항공,항공마일리지,온라인 여행사,여행/숙박,공항라운지,리조트,공항,공항라운지/PP,여행사,호텔,PP,라운지키,해외이용,저가항공,해외</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>medical</t>
+          <t>category_medical</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>약국,병원,동물병원,병원/약국,드럭스토어</t>
+          <t>약국,병원,병원/약국</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>others</t>
+          <t>category_financial_insurance</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>프리미엄,주유,인테리어,여행/숙박,국민행복,공항라운지,레저/스포츠,비즈니스,APP,해피포인트,하이브리드,정비,금융,제휴/PLCC,해외이용,네이버페이,수수료우대,PAYCO,간편결제,리조트,적립,경기관람,할인,공항,캐시백,렌탈,보험사,헤어,테마파크,해외,선택형,은행사,자동차,애완동물,프리미엄 서비스,CJ ONE,공항라운지/PP,주유소,멤버십포인트,바우처,여행사,골프,라운지키,지역,호텔,생활,보험,PP,피트니스,뷰티/피트니스,게임,무이자할부,삼성페이,카카오페이,OK캐쉬백,유의사항,화장품,연회비지원,무실적</t>
+          <t>금융,은행사,보험,보험사</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>category_others</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>애완동물,비즈니스,동물병원,지역,생활,렌탈,무실적</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[feat] add data and cors configure
</commit_message>
<xml_diff>
--- a/flask/static/data/result/categories.xlsx
+++ b/flask/static/data/result/categories.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>백화점,마트/편의점,온라인쇼핑,소셜커머스,해외직구,홈쇼핑,SPA브랜드,아울렛,대형마트,SSM,전통시장,면세점,모든가맹점,국내외가맹점,화장품,드럭스토어</t>
+          <t>쇼핑,백화점,마트/편의점,온라인쇼핑,소셜커머스,해외직구,홈쇼핑,SPA브랜드,아울렛,대형마트,SSM,전통시장,면세점,모든가맹점,국내외가맹점,화장품,드럭스토어</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>영화,공연/전시,문화센터,도서,음원사이트,영화/문화,디지털구독,골프</t>
+          <t>문화,여가,문화/여가,영화,공연/전시,문화센터,도서,음원사이트,영화/문화,디지털구독,골프</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>고속버스,항공권,기차,대중교통,렌터카,택시,교통</t>
+          <t>교통,고속버스,항공권,기차,대중교통,렌터카,택시,교통</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>주유,자동차,정비,주유소,충전소,하이패스,자동차/하이패스</t>
+          <t>자동차,주유,자동차,정비,주유소,충전소,하이패스,자동차/하이패스</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>카페,패밀리레스토랑,배달앱,베이커리,점심,저녁,일반음식점,패스트푸드,카페/디저트,푸드</t>
+          <t>음식,푸드,카페,패밀리레스토랑,배달앱,베이커리,점심,저녁,일반음식점,패스트푸드,카페/디저트,푸드</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>학습지,유치원,어린이집,학원,교육/육아</t>
+          <t>교육,학습지,유치원,어린이집,학원,교육/육아</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>공과금,공과금/렌탈,통신,KT,SKT,LGU+</t>
+          <t>주거,통신,주거/통신,공과금,공과금/렌탈,통신,KT,SKT,LGU+</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>진에어,대한항공,아시아나항공,제주항공,항공마일리지,온라인 여행사,여행/숙박,공항라운지,리조트,공항,공항라운지/PP,여행사,호텔,PP,라운지키,해외이용,저가항공,해외</t>
+          <t>여행,항공,여행/항공,진에어,대한항공,아시아나항공,제주항공,항공마일리지,온라인 여행사,여행/숙박,공항라운지,리조트,공항,공항라운지/PP,여행사,호텔,PP,라운지키,해외이용,저가항공,해외</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>약국,병원,병원/약국</t>
+          <t>의료,약국,병원,병원/약국</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>금융,은행사,보험,보험사</t>
+          <t>금융,금융/보험,은행사,보험,보험사</t>
         </is>
       </c>
     </row>

</xml_diff>